<commit_message>
Add note about plug-in-metadata
</commit_message>
<xml_diff>
--- a/extras/example-form/Example form - feature-demo-metadata.xlsx
+++ b/extras/example-form/Example form - feature-demo-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cking/github/surveycto-field-plug-ins/feature-demo-metadata/extras/example-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B110385-ECF7-FE41-A0FD-314FA61085A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BA8D93-2283-BB4C-9524-8A92E9D6FEB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19720" yWindow="11000" windowWidth="37560" windowHeight="23540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="460" windowWidth="37560" windowHeight="23540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="384">
   <si>
     <t>type</t>
   </si>
@@ -2620,6 +2620,21 @@
   </si>
   <si>
     <t>custom-feature-demo-metadata</t>
+  </si>
+  <si>
+    <t>show_metadata</t>
+  </si>
+  <si>
+    <t>get_metadata</t>
+  </si>
+  <si>
+    <t>plug-in-metadata(${name})</t>
+  </si>
+  <si>
+    <t>Metadata stored by field plug-ins can be accessed by other fields in your form by using the "plug-in-metadata()" function.&lt;br /&gt;&lt;br /&gt;Here is the value stored in the "name" field: &lt;strong&gt;${name}&lt;/strong&gt;&lt;br /&gt;And here is the metadata stored in that same field: &lt;strong&gt;${get_metadata}&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: calculate fields are evaluated whenever forms load or save, and whenever fields upon which they rely change. So in this example, just changing the metadata in the "name" field will not cause the calculate field to update. If you change the actual value stored in the "name" field, then the calculation will be re-evaluated and you will be able to see changes in the metadata reflected here. </t>
   </si>
 </sst>
 </file>
@@ -3068,7 +3083,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3217,6 +3232,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -3328,7 +3344,277 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
   </cellStyles>
-  <dxfs count="135">
+  <dxfs count="170">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6D9E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFBFB00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4785,18 +5071,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" style="9" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="19.83203125" style="9" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.5" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="62.83203125" style="10" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="23" style="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="12.6640625" style="9" customWidth="1" collapsed="1"/>
@@ -5063,142 +5349,314 @@
         <v>375</v>
       </c>
     </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="64" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="64" t="s">
+        <v>380</v>
+      </c>
+      <c r="C12"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12"/>
+      <c r="N12" s="9" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="272" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14"/>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="F1:F1048576 I1:I1048576 B1:C1048576">
-    <cfRule type="expression" dxfId="134" priority="84" stopIfTrue="1">
+  <conditionalFormatting sqref="F1:F13 I1:I13 B1:C13 B15:C1048576 I15:I1048576 F15:F1048576">
+    <cfRule type="expression" dxfId="169" priority="119" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:I1048576 O1:O1048576 B1:C1048576">
-    <cfRule type="expression" dxfId="133" priority="81" stopIfTrue="1">
+  <conditionalFormatting sqref="I1:I13 O1:O13 B1:C13 B15:C1048576 O15:O1048576 I15:I1048576">
+    <cfRule type="expression" dxfId="168" priority="116" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 B1:D1048576">
-    <cfRule type="expression" dxfId="132" priority="78" stopIfTrue="1">
+  <conditionalFormatting sqref="F1:F13 B1:D13 B15:D1048576 F15:F1048576">
+    <cfRule type="expression" dxfId="167" priority="113" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:H1048576 B1:D1048576">
-    <cfRule type="expression" dxfId="131" priority="76" stopIfTrue="1">
+  <conditionalFormatting sqref="G1:H13 B1:D13 B15:D1048576 G15:H1048576">
+    <cfRule type="expression" dxfId="166" priority="111" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:H1048576 B1:D1048576">
-    <cfRule type="expression" dxfId="130" priority="74" stopIfTrue="1">
+  <conditionalFormatting sqref="G1:H13 B1:D13 B15:D1048576 G15:H1048576">
+    <cfRule type="expression" dxfId="165" priority="109" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 B1:C1048576">
-    <cfRule type="expression" dxfId="129" priority="69" stopIfTrue="1">
+  <conditionalFormatting sqref="F1:F13 B1:C13 B15:C1048576 F15:F1048576">
+    <cfRule type="expression" dxfId="164" priority="104" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="128" priority="59" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B13 F1:F13 F15:F1048576 B15:B1048576">
+    <cfRule type="expression" dxfId="163" priority="94" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="127" priority="53" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C13 B15:C1048576">
+    <cfRule type="expression" dxfId="162" priority="88" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="90" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="92" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576 N1:N1048576">
-    <cfRule type="expression" dxfId="124" priority="51" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B13 N1:N13 N15:N1048576 B15:B1048576">
+    <cfRule type="expression" dxfId="159" priority="86" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 B1:C1048576">
-    <cfRule type="expression" dxfId="123" priority="49" stopIfTrue="1">
+  <conditionalFormatting sqref="F1:F13 B1:C13 B15:C1048576 F15:F1048576">
+    <cfRule type="expression" dxfId="158" priority="84" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 B1:C1048576">
-    <cfRule type="expression" dxfId="122" priority="45" stopIfTrue="1">
+  <conditionalFormatting sqref="F1:F13 B1:C13 B15:C1048576 F15:F1048576">
+    <cfRule type="expression" dxfId="157" priority="80" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="121" priority="43" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:C13 B15:C1048576">
+    <cfRule type="expression" dxfId="156" priority="78" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:W1048576">
-    <cfRule type="expression" dxfId="120" priority="37" stopIfTrue="1">
+  <conditionalFormatting sqref="A1:W13 A15:W1048576">
+    <cfRule type="expression" dxfId="155" priority="72" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="75" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="79" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="81" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="85" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="87" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="89" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="91" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="93" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="95" stopIfTrue="1">
       <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="98" stopIfTrue="1">
       <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="105" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="110" stopIfTrue="1">
       <formula>$A1="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="112" stopIfTrue="1">
       <formula>$A1="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="114" stopIfTrue="1">
       <formula>$A1="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="115" stopIfTrue="1">
       <formula>$A1="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="117" stopIfTrue="1">
       <formula>$A1="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="118" stopIfTrue="1">
       <formula>$A1="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="120" stopIfTrue="1">
       <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="101" priority="38" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B13 B15:B1048576">
+    <cfRule type="expression" dxfId="136" priority="73" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576 B1:B1048576">
-    <cfRule type="expression" dxfId="100" priority="36" stopIfTrue="1">
+  <conditionalFormatting sqref="F1:F13 B1:B13 B15:B1048576 F15:F1048576">
+    <cfRule type="expression" dxfId="135" priority="71" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14 I14 B14:C14">
+    <cfRule type="expression" dxfId="34" priority="34" stopIfTrue="1">
+      <formula>$A14="begin group"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14 O14 B14:C14">
+    <cfRule type="expression" dxfId="33" priority="31" stopIfTrue="1">
+      <formula>$A14="begin repeat"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14 B14:D14">
+    <cfRule type="expression" dxfId="32" priority="28" stopIfTrue="1">
+      <formula>$A14="text"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14:H14 B14:D14">
+    <cfRule type="expression" dxfId="31" priority="26" stopIfTrue="1">
+      <formula>$A14="integer"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14:H14 B14:D14">
+    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
+      <formula>$A14="decimal"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14 B14:C14">
+    <cfRule type="expression" dxfId="29" priority="22" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A14, 16)="select_multiple ", LEN($A14)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A14, 17)))), AND(LEFT($A14, 11)="select_one ", LEN($A14)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A14, 12)))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14 F14">
+    <cfRule type="expression" dxfId="28" priority="19" stopIfTrue="1">
+      <formula>OR($A14="audio audit", $A14="text audit", $A14="speed violations count", $A14="speed violations list", $A14="speed violations audit")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:C14">
+    <cfRule type="expression" dxfId="27" priority="13" stopIfTrue="1">
+      <formula>$A14="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="15" stopIfTrue="1">
+      <formula>$A14="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="17" stopIfTrue="1">
+      <formula>OR($A14="geopoint", $A14="geoshape", $A14="geotrace")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14 N14">
+    <cfRule type="expression" dxfId="24" priority="11" stopIfTrue="1">
+      <formula>OR($A14="calculate", $A14="calculate_here")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14 B14:C14">
+    <cfRule type="expression" dxfId="23" priority="9" stopIfTrue="1">
+      <formula>OR($A14="date", $A14="datetime")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14 B14:C14">
+    <cfRule type="expression" dxfId="22" priority="7" stopIfTrue="1">
+      <formula>$A14="image"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:C14">
+    <cfRule type="expression" dxfId="21" priority="5" stopIfTrue="1">
+      <formula>OR($A14="audio", $A14="video")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:W14">
+    <cfRule type="expression" dxfId="20" priority="2" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A14, 14)="sensor_stream ", LEN($A14)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A14, 15)))), AND(LEFT($A14, 17)="sensor_statistic ", LEN($A14)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A14, 18)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="4" stopIfTrue="1">
+      <formula>$A14="comments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="6" stopIfTrue="1">
+      <formula>OR($A14="audio", $A14="video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="8" stopIfTrue="1">
+      <formula>$A14="image"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="10" stopIfTrue="1">
+      <formula>OR($A14="date", $A14="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="12" stopIfTrue="1">
+      <formula>OR($A14="calculate", $A14="calculate_here")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="14" stopIfTrue="1">
+      <formula>$A14="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="16" stopIfTrue="1">
+      <formula>$A14="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="18" stopIfTrue="1">
+      <formula>OR($A14="geopoint", $A14="geoshape", $A14="geotrace")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="20" stopIfTrue="1">
+      <formula>OR($A14="audio audit", $A14="text audit", $A14="speed violations count", $A14="speed violations list", $A14="speed violations audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="21" stopIfTrue="1">
+      <formula>OR($A14="username", $A14="phonenumber", $A14="start", $A14="end", $A14="deviceid", $A14="subscriberid", $A14="simserial", $A14="caseid")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="23" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A14, 16)="select_multiple ", LEN($A14)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A14, 17)))), AND(LEFT($A14, 11)="select_one ", LEN($A14)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A14, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="25" stopIfTrue="1">
+      <formula>$A14="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="27" stopIfTrue="1">
+      <formula>$A14="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="29" stopIfTrue="1">
+      <formula>$A14="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="30" stopIfTrue="1">
+      <formula>$A14="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="32" stopIfTrue="1">
+      <formula>$A14="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="33" stopIfTrue="1">
+      <formula>$A14="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="35" stopIfTrue="1">
+      <formula>$A14="begin group"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
+      <formula>$A14="comments"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14 B14">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A14, 14)="sensor_stream ", LEN($A14)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A14, 15)))), AND(LEFT($A14, 17)="sensor_statistic ", LEN($A14)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A14, 18)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -5295,12 +5753,12 @@
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A2:H3 A5:H1997">
-    <cfRule type="expression" dxfId="99" priority="1">
+    <cfRule type="expression" dxfId="134" priority="1">
       <formula>NOT($A2=$A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:H4">
-    <cfRule type="expression" dxfId="98" priority="100">
+    <cfRule type="expression" dxfId="133" priority="100">
       <formula>NOT($A4=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5358,7 +5816,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2003261248</v>
+        <v>2006191651</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>358</v>
@@ -9194,348 +9652,348 @@
     <mergeCell ref="A83:B83"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:C5 H5 L5">
-    <cfRule type="expression" dxfId="97" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="97" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 L5 S5">
-    <cfRule type="expression" dxfId="96" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="94" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5 B5:F5">
-    <cfRule type="expression" dxfId="95" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="91" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="94" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="89" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5 B5:F5">
-    <cfRule type="expression" dxfId="93" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="87" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="92" priority="85" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="85" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 H5">
-    <cfRule type="expression" dxfId="91" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="82" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="90" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="76" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="78" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="80" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5 R5">
-    <cfRule type="expression" dxfId="87" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="74" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="86" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="72" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5 H5">
-    <cfRule type="expression" dxfId="85" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="70" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:C5">
-    <cfRule type="expression" dxfId="84" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="68" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:J5 L5:O5 Q5:S5 W5:AD5">
-    <cfRule type="expression" dxfId="83" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="67" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="69" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="71" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="73" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="75" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="77" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="79" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="79" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="81" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="83" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="83" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="84" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="86" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="88" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="90" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="92" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="93" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="95" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="96" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="98" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="65" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="66" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:V5">
-    <cfRule type="expression" dxfId="64" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="48" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="49" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="50" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="51" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="52" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="53" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="54" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="55" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="56" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="57" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="58" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="59" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="60" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="61" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="62" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="63" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="64" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="65" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="46" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="47" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="45" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="46" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="44" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="45" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="43" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="42" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="43" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="44" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="40" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="41" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="39" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="40" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="38" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="39" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="37" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="32" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="36" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="30" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="35" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="19" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="20" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="21" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="22" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="23" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="24" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="25" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="26" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="27" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="28" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="29" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="31" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="33" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="34" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="35" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="36" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="37" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="38" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P5">
-    <cfRule type="expression" dxfId="17" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="1" stopIfTrue="1">
       <formula>$A5="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="2" stopIfTrue="1">
       <formula>OR($A5="audio", $A5="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="3" stopIfTrue="1">
       <formula>$A5="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="4" stopIfTrue="1">
       <formula>OR($A5="date", $A5="datetime")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="5" stopIfTrue="1">
       <formula>OR($A5="calculate", $A5="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="6" stopIfTrue="1">
       <formula>$A5="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="7" stopIfTrue="1">
       <formula>$A5="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="8" stopIfTrue="1">
       <formula>$A5="geopoint"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="9" stopIfTrue="1">
       <formula>OR($A5="audio audit", $A5="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="10" stopIfTrue="1">
       <formula>OR($A5="phonenumber", $A5="start", $A5="end", $A5="deviceid", $A5="subscriberid", $A5="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="11" stopIfTrue="1">
       <formula>OR(AND(LEFT($A5, 16)="select_multiple ", LEN($A5)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A5, 17)))), AND(LEFT($A5, 11)="select_one ", LEN($A5)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A5, 12)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="12" stopIfTrue="1">
       <formula>$A5="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="13" stopIfTrue="1">
       <formula>$A5="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="14" stopIfTrue="1">
       <formula>$A5="text"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="15" stopIfTrue="1">
       <formula>$A5="end repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="16" stopIfTrue="1">
       <formula>$A5="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="17" stopIfTrue="1">
       <formula>$A5="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="18" stopIfTrue="1">
       <formula>$A5="begin group"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>